<commit_message>
add prodi & kuota dosen
</commit_message>
<xml_diff>
--- a/public/assets/files/Dosen.xlsx
+++ b/public/assets/files/Dosen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Coding\Monitoring TA\SIMONIKA\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC97CC07-52B8-4924-A6BC-27D52DBFA283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AB51B0-B98D-4B10-90D9-ADE6C1E7CBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="130">
   <si>
     <t>nip</t>
   </si>
@@ -403,6 +403,18 @@
   </si>
   <si>
     <t>Dusen Aseman RT 3/RW 2, Desa Bimorejo, Wongsorejo, Banyuwangi</t>
+  </si>
+  <si>
+    <t>program_studi</t>
+  </si>
+  <si>
+    <t>TRPL</t>
+  </si>
+  <si>
+    <t>TRK</t>
+  </si>
+  <si>
+    <t>BD</t>
   </si>
 </sst>
 </file>
@@ -506,7 +518,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -554,6 +566,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -839,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="H1" zoomScale="87" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +870,7 @@
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="88.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -876,6 +894,9 @@
       </c>
       <c r="G1" s="2" t="s">
         <v>104</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -906,6 +927,9 @@
       <c r="G2" s="17" t="s">
         <v>105</v>
       </c>
+      <c r="H2" s="19" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -929,6 +953,9 @@
       <c r="G3" s="17" t="s">
         <v>106</v>
       </c>
+      <c r="H3" s="19" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -952,6 +979,9 @@
       <c r="G4" s="17" t="s">
         <v>107</v>
       </c>
+      <c r="H4" s="19" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -975,6 +1005,9 @@
       <c r="G5" s="17" t="s">
         <v>108</v>
       </c>
+      <c r="H5" s="19" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -998,6 +1031,9 @@
       <c r="G6" s="17" t="s">
         <v>109</v>
       </c>
+      <c r="H6" s="19" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1021,6 +1057,9 @@
       <c r="G7" s="17" t="s">
         <v>110</v>
       </c>
+      <c r="H7" s="19" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1044,6 +1083,9 @@
       <c r="G8" s="17" t="s">
         <v>111</v>
       </c>
+      <c r="H8" s="19" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1067,6 +1109,9 @@
       <c r="G9" s="17" t="s">
         <v>112</v>
       </c>
+      <c r="H9" s="19" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -1090,6 +1135,9 @@
       <c r="G10" s="5" t="s">
         <v>113</v>
       </c>
+      <c r="H10" s="19" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1113,6 +1161,9 @@
       <c r="G11" s="5" t="s">
         <v>114</v>
       </c>
+      <c r="H11" s="19" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1136,6 +1187,9 @@
       <c r="G12" s="5" t="s">
         <v>115</v>
       </c>
+      <c r="H12" s="19" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1159,6 +1213,9 @@
       <c r="G13" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="H13" s="19" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -1182,6 +1239,9 @@
       <c r="G14" s="5" t="s">
         <v>117</v>
       </c>
+      <c r="H14" s="19" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -1205,6 +1265,9 @@
       <c r="G15" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="H15" s="19" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1228,8 +1291,11 @@
       <c r="G16" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>5099006</v>
       </c>
@@ -1251,8 +1317,11 @@
       <c r="G17" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>27029204</v>
       </c>
@@ -1274,8 +1343,11 @@
       <c r="G18" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>27088704</v>
       </c>
@@ -1297,8 +1369,11 @@
       <c r="G19" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>21099202</v>
       </c>
@@ -1320,8 +1395,11 @@
       <c r="G20" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
@@ -1343,8 +1421,11 @@
       <c r="G21" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>523038903</v>
       </c>
@@ -1366,8 +1447,11 @@
       <c r="G22" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>711039101</v>
       </c>
@@ -1388,6 +1472,9 @@
       </c>
       <c r="G23" s="5" t="s">
         <v>125</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>